<commit_message>
Added links to components
</commit_message>
<xml_diff>
--- a/data/components.xlsx
+++ b/data/components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cverhoosel/Documents/2_Education/4CBLA30_Energy_Storage_and_Transport/Energy-Storage-and-Transport.github.io/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl.sharepoint.com/sites/EST2020/Shared Documents/General/Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF8AE6ED-5DE8-AE47-95B8-9E04A27CF08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F3C9C8A-DF2C-4C76-8484-593F40E7B29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{B795D2B2-84D1-4D57-9EC8-769A1489C68E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="177">
   <si>
     <t>Name</t>
   </si>
@@ -97,6 +97,9 @@
     <t>Arduino prototyping board</t>
   </si>
   <si>
+    <t>(documentation,https://docs.arduino.cc/hardware/uno-rev3/)</t>
+  </si>
+  <si>
     <t>On board</t>
   </si>
   <si>
@@ -139,6 +142,9 @@
     <t xml:space="preserve">DS18B20 </t>
   </si>
   <si>
+    <t>(specs,https://www.tinytronics.nl/product_files/000946_DS18B20_datasheet.pdf)</t>
+  </si>
+  <si>
     <t>EST-S0001</t>
   </si>
   <si>
@@ -148,6 +154,9 @@
     <t>measure water flow</t>
   </si>
   <si>
+    <t>(specs, https://www.tinytronics.nl/en/sensors/liquid/yf-s401-water-flow-sensor)</t>
+  </si>
+  <si>
     <t>EST-S0002</t>
   </si>
   <si>
@@ -157,13 +166,16 @@
     <t>measure distance</t>
   </si>
   <si>
+    <t>(specs, https://www.tinytronics.nl/en/sensors/distance/ultrasonic-sensor-hy-srf05)</t>
+  </si>
+  <si>
     <t>EST-S0003</t>
   </si>
   <si>
     <t>air flow sensor ( PF2A521-F03-1 )</t>
   </si>
   <si>
-    <t>PF2A521.pdf</t>
+    <t>(specs,PF2A521.pdf)</t>
   </si>
   <si>
     <t>SMC</t>
@@ -175,24 +187,36 @@
     <t>SMC pressure sensor</t>
   </si>
   <si>
+    <t>(specs,PSE570.pdf)</t>
+  </si>
+  <si>
     <t>EST-S0005</t>
   </si>
   <si>
     <t>power sensor for DC Motor</t>
   </si>
   <si>
+    <t>(specs, https://nl.aliexpress.com/item/1005003819758065.html?srcSns=sns_Copy&amp;spreadType=socialShare&amp;bizType=ProductDetail&amp;social_params=60501622654&amp;aff_fcid=8b74fdab2db5447b8ea76a0f14118359-1713377130251-01662-_EQtoqmV&amp;tt=MG&amp;aff_fsk=_EQtoqmV&amp;aff_platform=default&amp;sk=_EQtoqmV&amp;aff_trace_key=8b74fdab2db5447b8ea76a0f14118359-1713377130251-01662-_EQtoqmV&amp;shareId=60501622654&amp;businessType=ProductDetail&amp;platform=AE&amp;terminal_id=18a73b87c1d841e295dd3dd0d265d371&amp;afSmartRedirect=y&amp;gatewayAdapt=glo2nld)</t>
+  </si>
+  <si>
     <t>EST-S0006</t>
   </si>
   <si>
     <t>light slot sensor</t>
   </si>
   <si>
+    <t>(specs,https://www.tinytronics.nl/en/sensors/optical/light-slots/licht-slot-sensor-module-10mm)</t>
+  </si>
+  <si>
     <t>EST-S0007</t>
   </si>
   <si>
     <t>acceleration sensor</t>
   </si>
   <si>
+    <t>(specs,https://www.tinytronics.nl/en/sensors/acceleration-rotation/adxl345-digital-3-axis-accelerometer-module-v2)</t>
+  </si>
+  <si>
     <t>EST-S0008</t>
   </si>
   <si>
@@ -415,7 +439,7 @@
     <t>Motor with adjustable gear ratios. Max 24v</t>
   </si>
   <si>
-    <t>on board</t>
+    <t>(specs, https://nl.rs-online.com/web/p/dc-motors/2389822)</t>
   </si>
   <si>
     <t>RS</t>
@@ -545,19 +569,13 @@
   </si>
   <si>
     <t>kleinpvc tankje</t>
-  </si>
-  <si>
-    <t>(documentation,https://docs.arduino.cc/hardware/uno-rev3/)</t>
-  </si>
-  <si>
-    <t>(specsheet,https://www.tinytronics.nl/product_files/000946_DS18B20_datasheet.pdf)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,16 +610,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0E6F5"/>
+        <bgColor rgb="FFC0E6F5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -609,17 +639,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF44B3E1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF44B3E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,10 +729,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1040,30 +1079,30 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="118" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1126,24 +1165,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>169</v>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -1169,18 +1208,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <f>80+27</f>
@@ -1204,21 +1243,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5">
         <f>20+1</f>
@@ -1236,12 +1275,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6">
         <v>19</v>
@@ -1258,24 +1297,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>170</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7">
         <v>18</v>
@@ -1291,21 +1330,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G8">
         <f xml:space="preserve"> 20 + 12</f>
@@ -1323,15 +1365,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
@@ -1342,21 +1387,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G10">
         <v>5</v>
@@ -1370,15 +1415,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G11">
         <f xml:space="preserve"> 40+1</f>
@@ -1396,15 +1444,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G12">
         <f>20+1</f>
@@ -1422,15 +1476,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G13">
         <v>24</v>
@@ -1447,15 +1507,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G14">
         <v>45</v>
@@ -1471,15 +1537,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G15">
         <f>40+28</f>
@@ -1500,15 +1566,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G16">
         <f>40+38</f>
@@ -1529,15 +1595,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G17">
         <f>40+32</f>
@@ -1555,15 +1621,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="G18">
         <f>20+16</f>
@@ -1581,15 +1647,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G19">
         <f>80+29</f>
@@ -1607,15 +1673,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G20">
         <f>40+18</f>
@@ -1633,15 +1699,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G21">
         <f>40+11</f>
@@ -1659,15 +1725,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="G22">
         <f>40+10</f>
@@ -1685,15 +1751,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G23">
         <f>80+2</f>
@@ -1714,15 +1780,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G24">
         <f>80+24</f>
@@ -1743,15 +1809,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F25" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G25">
         <f>80+8</f>
@@ -1772,15 +1838,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G26">
         <f>100+12</f>
@@ -1801,15 +1867,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G27">
         <f>80+22</f>
@@ -1830,15 +1896,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
@@ -1851,15 +1917,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F29" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
@@ -1875,15 +1941,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F30" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G30">
         <f>80+35</f>
@@ -1904,15 +1970,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F31" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="G31">
         <f xml:space="preserve"> 40 + 4</f>
@@ -1933,15 +1999,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F32" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="H32">
         <f t="shared" si="0"/>
@@ -1952,15 +2018,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E33" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F33" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
@@ -1971,15 +2037,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E34" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F34" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
@@ -1990,18 +2056,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E35" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F35" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G35">
         <f xml:space="preserve"> 20 + 16</f>
@@ -2019,15 +2085,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F36" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G36">
         <v>34</v>
@@ -2044,18 +2110,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E37" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F37" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G37">
         <f xml:space="preserve"> 40 + 6</f>
@@ -2073,12 +2139,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F38" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G38">
         <v>2</v>
@@ -2092,18 +2158,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F39" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="G39">
         <v>25</v>
@@ -2120,15 +2186,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F40" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G40">
         <f>20+8</f>
@@ -2145,12 +2211,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F41" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="G41">
         <f>20+13</f>
@@ -2167,16 +2233,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" s="4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B42" s="1"/>
       <c r="E42" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F42" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="G42">
         <v>21</v>
@@ -2192,12 +2258,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="F43" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="H43">
         <f t="shared" si="0"/>
@@ -2208,12 +2274,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="F44" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -2226,12 +2292,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="F45" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G45">
         <v>20</v>
@@ -2244,12 +2310,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F46" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="G46">
         <v>5</v>
@@ -2263,24 +2329,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E47" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F47" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G47">
         <v>24</v>
@@ -2297,15 +2363,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E48" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F48" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="G48">
         <v>45</v>
@@ -2322,15 +2388,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E49" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="F49" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="G49">
         <v>22</v>
@@ -2347,12 +2413,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F50" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G50">
         <f xml:space="preserve"> 20 + 10</f>
@@ -2366,12 +2432,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="F51" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="G51">
         <v>21</v>
@@ -2387,12 +2453,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F52" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="H52">
         <f t="shared" ref="H52:H60" si="3">G52-J52-I52</f>
@@ -2403,12 +2469,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F53" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="H53">
         <f t="shared" si="3"/>
@@ -2419,12 +2485,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F54" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H54">
         <f t="shared" si="3"/>
@@ -2438,12 +2504,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="F55" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="H55">
         <f t="shared" si="3"/>
@@ -2457,12 +2523,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="F56" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="H56">
         <f t="shared" si="3"/>
@@ -2476,12 +2542,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F57" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H57">
         <f t="shared" si="3"/>
@@ -2495,12 +2561,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F58" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="H58">
         <f t="shared" si="3"/>
@@ -2514,12 +2580,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="F59" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="H59">
         <f t="shared" si="3"/>
@@ -2533,12 +2599,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="F60" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H60">
         <f t="shared" si="3"/>
@@ -2580,7 +2646,7 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1" display="https://www.bitsandparts.nl/Temperatuursensor-1-wire-Waterdicht-Dallas-DS18B20-2-meter-p109707" xr:uid="{9FFC9E7B-A3BC-41DC-9E4A-9E1829241AA9}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://store.arduino.cc/en-nl/products/arduino-uno-rev3?srsltid=AfmBOoqV6nKlv28zGLP7TRCnfL7lt0ZwXx8Yo48ohQyyKPPxEWplbDm5" xr:uid="{4CE510F4-6ECC-423C-9EBB-97213A3C5F59}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{A50BE7E1-47D7-462A-B893-02FD9AA08531}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -2598,9 +2664,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2608,15 +2674,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2624,7 +2690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2645,63 +2711,63 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F2" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="G2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="G3" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H3" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2710,17 +2776,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c43a8398-59d6-4544-8889-d61e38456917">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5290365f-c8d6-40d0-b44a-6be08a8a62f3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F5CB8A00F1A0841B3F9E89D33680BD0" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c000b4385f70b7b1f84268cc1d8b6f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c43a8398-59d6-4544-8889-d61e38456917" xmlns:ns3="5290365f-c8d6-40d0-b44a-6be08a8a62f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66dbeb20f29d81400e6a07d4788d4730" ns2:_="" ns3:_="">
     <xsd:import namespace="c43a8398-59d6-4544-8889-d61e38456917"/>
@@ -2975,7 +3030,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2984,46 +3039,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c43a8398-59d6-4544-8889-d61e38456917">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5290365f-c8d6-40d0-b44a-6be08a8a62f3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17D6B607-A9B3-43F0-AF54-4344976BB527}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5290365f-c8d6-40d0-b44a-6be08a8a62f3"/>
-    <ds:schemaRef ds:uri="c43a8398-59d6-4544-8889-d61e38456917"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED5F3FA2-F157-4A54-88A9-DA8FEABFC56D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED5F3FA2-F157-4A54-88A9-DA8FEABFC56D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c43a8398-59d6-4544-8889-d61e38456917"/>
-    <ds:schemaRef ds:uri="5290365f-c8d6-40d0-b44a-6be08a8a62f3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84604F91-3C59-4AE5-92E7-93618F763177}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84604F91-3C59-4AE5-92E7-93618F763177}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17D6B607-A9B3-43F0-AF54-4344976BB527}"/>
 </file>
</xml_diff>

<commit_message>
Added gravity V/A lib
</commit_message>
<xml_diff>
--- a/data/components.xlsx
+++ b/data/components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl.sharepoint.com/sites/EST2020/Shared Documents/General/Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="417" documentId="13_ncr:1_{A2AE6154-438B-2B4E-97D2-09BB0C0E94FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACF31467-76CC-480D-AB82-676A931DC92B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E56573D-CC22-437F-BC87-D2DB009C66CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B795D2B2-84D1-4D57-9EC8-769A1489C68E}"/>
   </bookViews>
@@ -196,10 +196,10 @@
     <t>EST-S0005</t>
   </si>
   <si>
-    <t>power sensor for DC Motor</t>
-  </si>
-  <si>
-    <t>(specs, https://www.tinytronics.nl/nl/sensoren/stroom-spanning/ina3221-i2c-dc-stroom-en-spanningssensor-module-1.6a-3-kanalen);(code,https://gist.github.com/CVerhoosel/3b5a952a7eaee7f8d63b1722fe6c8f3f)</t>
+    <t>volatge and current sensor for DC Motor</t>
+  </si>
+  <si>
+    <t>(specs, https://www.tinytronics.nl/nl/sensoren/stroom-spanning/ina3221-i2c-dc-stroom-en-spanningssensor-module-1.6a-3-kanalen);(code,https://gist.github.com/CVerhoosel/3b5a952a7eaee7f8d63b1722fe6c8f3f);(lib,SDL_Arduino_INA3221.zip)</t>
   </si>
   <si>
     <t>EST-S0006</t>
@@ -538,7 +538,7 @@
     <t>Temperature Sensor Connector (jack to Screw-Terminal)</t>
   </si>
   <si>
-    <t>(Diagram,DS18B20_Connector_Diagram.png)</t>
+    <t>(diagram,DS18B20_Connector_Diagram.png)</t>
   </si>
   <si>
     <t>EST-T0006</t>
@@ -754,10 +754,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DC69B98-0BD3-6F4A-8A7B-E3E9EDB4ADF1}" name="Table1" displayName="Table1" ref="A1:N60" totalsRowShown="0">
   <autoFilter ref="A1:N60" xr:uid="{7DC69B98-0BD3-6F4A-8A7B-E3E9EDB4ADF1}">
-    <filterColumn colId="13">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="1"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
@@ -1105,7 +1105,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="118" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C61" sqref="C61"/>
+      <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" hidden="1">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" hidden="1">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>133</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>138</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:14" hidden="1">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>146</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" hidden="1">
       <c r="A54" t="s">
         <v>154</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" hidden="1">
       <c r="A55" t="s">
         <v>157</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" hidden="1">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" hidden="1">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" hidden="1">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" hidden="1">
       <c r="A59" t="s">
         <v>165</v>
       </c>
@@ -2826,15 +2826,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F5CB8A00F1A0841B3F9E89D33680BD0" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c000b4385f70b7b1f84268cc1d8b6f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c43a8398-59d6-4544-8889-d61e38456917" xmlns:ns3="5290365f-c8d6-40d0-b44a-6be08a8a62f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66dbeb20f29d81400e6a07d4788d4730" ns2:_="" ns3:_="">
     <xsd:import namespace="c43a8398-59d6-4544-8889-d61e38456917"/>
@@ -3089,6 +3080,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3101,11 +3101,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84604F91-3C59-4AE5-92E7-93618F763177}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED5F3FA2-F157-4A54-88A9-DA8FEABFC56D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED5F3FA2-F157-4A54-88A9-DA8FEABFC56D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84604F91-3C59-4AE5-92E7-93618F763177}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>